<commit_message>
removed econ_q from model inputs
</commit_message>
<xml_diff>
--- a/data/PH_Econ_Q.xlsx
+++ b/data/PH_Econ_Q.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/btiu/Documents/Tweets/Gavin/TweetsNowcast/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benedict-t/Documents/tweets_parallel/TweetsNowcast/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA3E383-E9FA-3E46-82DF-94C82BB27D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC55265-81D7-8D4D-9C06-6BE027DBEA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="27020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="1133">
   <si>
     <t>date</t>
   </si>
@@ -3318,9 +3321,6 @@
     <t>26</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>367521847</t>
   </si>
   <si>
@@ -3427,13 +3427,30 @@
   </si>
   <si>
     <t>GDP</t>
+  </si>
+  <si>
+    <t>GDP Growth</t>
+  </si>
+  <si>
+    <t>GDPG_Est_YoY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3459,13 +3476,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3803,19 +3828,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R93"/>
+  <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="26.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3826,7 +3851,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -3870,8 +3895,11 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3918,7 +3946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3965,7 +3993,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -4012,7 +4040,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -4059,7 +4087,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -4115,7 +4143,7 @@
         <v>24.49042772214672</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -4171,7 +4199,7 @@
         <v>-274.83686844560884</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -4227,7 +4255,7 @@
         <v>-162.95346494023798</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -4283,7 +4311,7 @@
         <v>-78.560645977013081</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -4339,7 +4367,7 @@
         <v>-73.169205961771922</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -4395,7 +4423,7 @@
         <v>-14.304185253082693</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>131</v>
       </c>
@@ -4451,7 +4479,7 @@
         <v>24.900029029401228</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>142</v>
       </c>
@@ -4507,7 +4535,7 @@
         <v>-379.35372774289624</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -4563,7 +4591,7 @@
         <v>-663.4307230496197</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>166</v>
       </c>
@@ -4619,7 +4647,7 @@
         <v>18.254845111223478</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>178</v>
       </c>
@@ -5571,7 +5599,7 @@
         <v>11.582399454873469</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>376</v>
       </c>
@@ -5627,7 +5655,7 @@
         <v>153.45386915149527</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>388</v>
       </c>
@@ -5683,7 +5711,7 @@
         <v>-607.89828036534573</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>399</v>
       </c>
@@ -5739,7 +5767,7 @@
         <v>71.852448438513818</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>411</v>
       </c>
@@ -5795,7 +5823,7 @@
         <v>47.487142692426083</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>422</v>
       </c>
@@ -5851,7 +5879,7 @@
         <v>-89.166412659095883</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>434</v>
       </c>
@@ -5907,7 +5935,7 @@
         <v>10.308901283282724</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>445</v>
       </c>
@@ -5963,7 +5991,7 @@
         <v>21.816047491874325</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>457</v>
       </c>
@@ -6019,7 +6047,7 @@
         <v>-40.281040859063147</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>469</v>
       </c>
@@ -6075,7 +6103,7 @@
         <v>829.97336481075979</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>481</v>
       </c>
@@ -6130,8 +6158,11 @@
       <c r="R42">
         <v>74.077118859952918</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S42" s="1">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>493</v>
       </c>
@@ -6186,8 +6217,11 @@
       <c r="R43">
         <v>39.077182529621304</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S43" s="1">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>504</v>
       </c>
@@ -6242,8 +6276,11 @@
       <c r="R44">
         <v>-41.340489020593679</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S44" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>516</v>
       </c>
@@ -6298,8 +6335,11 @@
       <c r="R45">
         <v>138.6720657245296</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S45" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>527</v>
       </c>
@@ -6354,8 +6394,11 @@
       <c r="R46">
         <v>88.141122519589047</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S46" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>538</v>
       </c>
@@ -6410,8 +6453,11 @@
       <c r="R47">
         <v>-4.3825049831712475</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S47" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>550</v>
       </c>
@@ -6466,8 +6512,11 @@
       <c r="R48">
         <v>291.29800097321561</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S48" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>561</v>
       </c>
@@ -6522,8 +6571,11 @@
       <c r="R49">
         <v>41.727947845531219</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S49" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>573</v>
       </c>
@@ -6578,8 +6630,11 @@
       <c r="R50">
         <v>-30.334172141081805</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S50" s="1">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>584</v>
       </c>
@@ -6634,8 +6689,11 @@
       <c r="R51">
         <v>10.756351172863733</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S51" s="1">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>596</v>
       </c>
@@ -6690,8 +6748,11 @@
       <c r="R52">
         <v>9.707499744763167</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S52" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>607</v>
       </c>
@@ -6746,8 +6807,11 @@
       <c r="R53">
         <v>8.0710661164796988</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S53" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>618</v>
       </c>
@@ -6802,8 +6866,11 @@
       <c r="R54">
         <v>21.433893887424773</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S54" s="1">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>629</v>
       </c>
@@ -6858,8 +6925,11 @@
       <c r="R55">
         <v>34.705313418552166</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S55" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>640</v>
       </c>
@@ -6914,8 +6984,11 @@
       <c r="R56">
         <v>39.862574068641017</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S56" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>651</v>
       </c>
@@ -6970,8 +7043,11 @@
       <c r="R57">
         <v>1.5880155576538091</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S57" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>662</v>
       </c>
@@ -7026,8 +7102,11 @@
       <c r="R58">
         <v>44.264664444441451</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S58" s="1">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>673</v>
       </c>
@@ -7082,8 +7161,11 @@
       <c r="R59">
         <v>-19.63586287047799</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S59" s="1">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>684</v>
       </c>
@@ -7138,8 +7220,11 @@
       <c r="R60">
         <v>12.171687153009852</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S60" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>696</v>
       </c>
@@ -7194,8 +7279,11 @@
       <c r="R61">
         <v>-20.050127652530826</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S61" s="1">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>708</v>
       </c>
@@ -7250,8 +7338,11 @@
       <c r="R62">
         <v>26.421798494888769</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S62" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>720</v>
       </c>
@@ -7306,8 +7397,11 @@
       <c r="R63">
         <v>54.819300013023742</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S63" s="1">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>731</v>
       </c>
@@ -7362,8 +7456,11 @@
       <c r="R64">
         <v>62.179349371185133</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S64" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>743</v>
       </c>
@@ -7418,8 +7515,11 @@
       <c r="R65">
         <v>97.793616065465741</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S65" s="1">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>755</v>
       </c>
@@ -7474,8 +7574,11 @@
       <c r="R66">
         <v>51.801189744695542</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S66" s="1">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>767</v>
       </c>
@@ -7530,8 +7633,11 @@
       <c r="R67">
         <v>100.89800006254532</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S67" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>779</v>
       </c>
@@ -7586,8 +7692,11 @@
       <c r="R68">
         <v>36.470145511311785</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S68" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>791</v>
       </c>
@@ -7642,8 +7751,11 @@
       <c r="R69">
         <v>51.390383945645638</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S69" s="1">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>803</v>
       </c>
@@ -7698,8 +7810,11 @@
       <c r="R70">
         <v>28.183209394109245</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S70" s="1">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>814</v>
       </c>
@@ -7754,8 +7869,11 @@
       <c r="R71">
         <v>23.393842361862085</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S71" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>825</v>
       </c>
@@ -7810,8 +7928,11 @@
       <c r="R72">
         <v>18.136363629066242</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S72" s="1">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>836</v>
       </c>
@@ -7866,8 +7987,11 @@
       <c r="R73">
         <v>20.010747874365038</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S73" s="1">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>848</v>
       </c>
@@ -7922,8 +8046,11 @@
       <c r="R74">
         <v>21.779704030977026</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S74" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>860</v>
       </c>
@@ -7978,8 +8105,11 @@
       <c r="R75">
         <v>46.133969853223405</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S75" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>872</v>
       </c>
@@ -8034,8 +8164,11 @@
       <c r="R76">
         <v>45.144666679160459</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S76" s="1">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>883</v>
       </c>
@@ -8090,8 +8223,11 @@
       <c r="R77">
         <v>25.199170951198411</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S77" s="1">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>895</v>
       </c>
@@ -8146,8 +8282,11 @@
       <c r="R78">
         <v>21.657259436154998</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S78" s="1">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>907</v>
       </c>
@@ -8202,8 +8341,11 @@
       <c r="R79">
         <v>-1.2312754125420258</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S79" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>918</v>
       </c>
@@ -8258,8 +8400,11 @@
       <c r="R80">
         <v>11.641732394117611</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S80" s="1">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>929</v>
       </c>
@@ -8314,8 +8459,11 @@
       <c r="R81">
         <v>0.55505370434057832</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S81" s="1">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>941</v>
       </c>
@@ -8370,8 +8518,11 @@
       <c r="R82">
         <v>-19.387168188573568</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S82" s="1">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>952</v>
       </c>
@@ -8426,8 +8577,11 @@
       <c r="R83">
         <v>-47.680758422526324</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S83" s="1">
+        <v>-16.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>964</v>
       </c>
@@ -8482,8 +8636,11 @@
       <c r="R84">
         <v>-38.980817704933131</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S84" s="1">
+        <v>-11.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>976</v>
       </c>
@@ -8538,8 +8695,11 @@
       <c r="R85">
         <v>-30.653462004829947</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S85" s="1">
+        <v>-8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>988</v>
       </c>
@@ -8594,8 +8754,11 @@
       <c r="R86">
         <v>0.89817846035804838</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S86" s="1">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1000</v>
       </c>
@@ -8650,8 +8813,11 @@
       <c r="R87">
         <v>99.073803050409097</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S87" s="1">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>1011</v>
       </c>
@@ -8706,8 +8872,11 @@
       <c r="R88">
         <v>61.588153655554621</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S88" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>1022</v>
       </c>
@@ -8762,8 +8931,11 @@
       <c r="R89">
         <v>74.047785748772526</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S89" s="1">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>1033</v>
       </c>
@@ -8818,8 +8990,11 @@
       <c r="R90">
         <v>46.19452006346377</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S90" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1044</v>
       </c>
@@ -8874,8 +9049,11 @@
       <c r="R91">
         <v>50.520233429225058</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S91" s="1">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>1055</v>
       </c>
@@ -8930,8 +9108,11 @@
       <c r="R92">
         <v>53.378476708729558</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S92" s="1">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>1066</v>
       </c>
@@ -8985,6 +9166,9 @@
       </c>
       <c r="R93">
         <v>-2.1903883462240428</v>
+      </c>
+      <c r="S93" s="1">
+        <v>7.2</v>
       </c>
     </row>
   </sheetData>
@@ -8997,10 +9181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9066,15 +9250,15 @@
         <v>1094</v>
       </c>
       <c r="J2" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B3" t="s">
         <v>1096</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1097</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -9083,7 +9267,7 @@
         <v>1089</v>
       </c>
       <c r="E3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F3" t="s">
         <v>1091</v>
@@ -9098,18 +9282,18 @@
         <v>1094</v>
       </c>
       <c r="J3" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B4" t="s">
         <v>1099</v>
       </c>
-      <c r="B4" t="s">
-        <v>1100</v>
-      </c>
       <c r="C4" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="D4" t="s">
         <v>1089</v>
@@ -9126,19 +9310,19 @@
       <c r="H4" t="s">
         <v>1093</v>
       </c>
-      <c r="I4" t="s">
-        <v>1094</v>
+      <c r="I4" s="2">
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B5" t="s">
         <v>1099</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1100</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -9162,15 +9346,15 @@
         <v>1094</v>
       </c>
       <c r="J5" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B6" t="s">
         <v>1102</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1103</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9179,7 +9363,7 @@
         <v>1089</v>
       </c>
       <c r="E6" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="F6" t="s">
         <v>1091</v>
@@ -9194,15 +9378,15 @@
         <v>1094</v>
       </c>
       <c r="J6" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B7" t="s">
         <v>1105</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1106</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -9211,10 +9395,10 @@
         <v>1089</v>
       </c>
       <c r="E7" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F7" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G7" t="s">
         <v>1092</v>
@@ -9226,15 +9410,15 @@
         <v>1094</v>
       </c>
       <c r="J7" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B8" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -9243,7 +9427,7 @@
         <v>1089</v>
       </c>
       <c r="E8" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F8" t="s">
         <v>1091</v>
@@ -9258,15 +9442,15 @@
         <v>1094</v>
       </c>
       <c r="J8" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B9" t="s">
         <v>1109</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1110</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -9275,10 +9459,10 @@
         <v>1089</v>
       </c>
       <c r="E9" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F9" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G9" t="s">
         <v>1092</v>
@@ -9290,15 +9474,15 @@
         <v>1094</v>
       </c>
       <c r="J9" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B10" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -9307,7 +9491,7 @@
         <v>1089</v>
       </c>
       <c r="E10" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F10" t="s">
         <v>1091</v>
@@ -9322,15 +9506,15 @@
         <v>1094</v>
       </c>
       <c r="J10" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B11" t="s">
         <v>1112</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1113</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -9339,10 +9523,10 @@
         <v>1089</v>
       </c>
       <c r="E11" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F11" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G11" t="s">
         <v>1092</v>
@@ -9354,15 +9538,15 @@
         <v>1094</v>
       </c>
       <c r="J11" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B12" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -9371,7 +9555,7 @@
         <v>1089</v>
       </c>
       <c r="E12" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F12" t="s">
         <v>1091</v>
@@ -9386,15 +9570,15 @@
         <v>1094</v>
       </c>
       <c r="J12" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B13" t="s">
         <v>1115</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1116</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -9403,10 +9587,10 @@
         <v>1089</v>
       </c>
       <c r="E13" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F13" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G13" t="s">
         <v>1092</v>
@@ -9418,15 +9602,15 @@
         <v>1094</v>
       </c>
       <c r="J13" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B14" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -9435,7 +9619,7 @@
         <v>1089</v>
       </c>
       <c r="E14" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F14" t="s">
         <v>1091</v>
@@ -9450,15 +9634,15 @@
         <v>1094</v>
       </c>
       <c r="J14" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B15" t="s">
         <v>1120</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1121</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -9467,7 +9651,7 @@
         <v>1089</v>
       </c>
       <c r="E15" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F15" t="s">
         <v>1091</v>
@@ -9482,15 +9666,15 @@
         <v>1094</v>
       </c>
       <c r="J15" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B16" t="s">
         <v>1122</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1123</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -9499,30 +9683,30 @@
         <v>1089</v>
       </c>
       <c r="E16" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="F16" t="s">
         <v>1091</v>
       </c>
       <c r="G16" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H16" t="s">
         <v>1125</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>1126</v>
       </c>
-      <c r="I16" t="s">
-        <v>1127</v>
-      </c>
       <c r="J16" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B17" t="s">
         <v>1128</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1129</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -9531,10 +9715,10 @@
         <v>1089</v>
       </c>
       <c r="E17" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F17" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G17" t="s">
         <v>1092</v>
@@ -9546,15 +9730,15 @@
         <v>1094</v>
       </c>
       <c r="J17" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B18" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -9563,7 +9747,7 @@
         <v>1089</v>
       </c>
       <c r="E18" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F18" t="s">
         <v>1091</v>
@@ -9578,13 +9762,39 @@
         <v>1094</v>
       </c>
       <c r="J18" t="s">
-        <v>1095</v>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E19" s="2">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1092</v>
+      </c>
+      <c r="I19" s="2">
+        <v>26</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A5:J18 A1:J3" numberStoredAsText="1"/>
+    <ignoredError sqref="A5:J7 A1:J1 A3:I3 B2:I2 B18:I18 B17:J17 A9:J9 A8:I8 A11:J11 A10:I10 A13:J13 A12:I12 A16:J16 A15:I15 A14:I14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to 41 day lags
</commit_message>
<xml_diff>
--- a/data/PH_Econ_Q.xlsx
+++ b/data/PH_Econ_Q.xlsx
@@ -5805,7 +5805,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I2" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J2" t="str">
         <v>0</v>
@@ -5837,7 +5837,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I3" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J3" t="str">
         <v>0</v>
@@ -5965,7 +5965,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I7" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J7" t="str">
         <v>0</v>
@@ -5997,7 +5997,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I8" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J8" t="str">
         <v>0</v>
@@ -6029,7 +6029,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I9" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J9" t="str">
         <v>0</v>
@@ -6061,7 +6061,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I10" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J10" t="str">
         <v>0</v>
@@ -6093,7 +6093,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I11" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J11" t="str">
         <v>0</v>
@@ -6125,7 +6125,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I12" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J12" t="str">
         <v>0</v>
@@ -6157,7 +6157,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I13" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J13" t="str">
         <v>0</v>
@@ -6189,7 +6189,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I14" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J14" t="str">
         <v>0</v>
@@ -6221,7 +6221,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I15" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J15" t="str">
         <v>0</v>
@@ -6253,7 +6253,7 @@
         <v>2023-03-09</v>
       </c>
       <c r="I16" t="str">
-        <v>-22</v>
+        <v>39</v>
       </c>
       <c r="J16" t="str">
         <v>0</v>
@@ -6285,7 +6285,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I17" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J17" t="str">
         <v>0</v>
@@ -6317,7 +6317,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="I18" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J18" t="str">
         <v>0</v>
@@ -6343,7 +6343,7 @@
         <v>2022-12-01</v>
       </c>
       <c r="I19" t="str">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J19" t="str">
         <v>0</v>

</xml_diff>